<commit_message>
Fix move route button - change type from button to submit
Co-authored-by: Fernandx7 <104953114+Fernandx7@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/planilhas/coleta_campo_grande.xlsx
+++ b/planilhas/coleta_campo_grande.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,95 +458,99 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">centauro park shopping </t>
+          <t xml:space="preserve">bazar da babi </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Estr. do Monteiro, 1200</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t xml:space="preserve">Estr. do Monteiro, 1200 </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Loja 105 E entrada B</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">bazar da babi </t>
+          <t xml:space="preserve">magic gril </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Estr. do Monteiro, 1200 </t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Loja 105 E entrada B</t>
-        </is>
-      </c>
+          <t>Rua Aricuri, 649</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">magic gril </t>
+          <t xml:space="preserve">melanina </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rua Aricuri, 649</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t xml:space="preserve">R Soldado Felisbino dos Santos, 97 </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sobreloja </t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">melanina </t>
+          <t xml:space="preserve">centauro west </t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">R Soldado Felisbino dos Santos, 97 </t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sobreloja </t>
-        </is>
-      </c>
+          <t xml:space="preserve"> Estr. do Mendanha, 555</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">centauro west </t>
+          <t xml:space="preserve">brecho kids </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Estr. do Mendanha, 555</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t xml:space="preserve">Av. das Américas, 29470 </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>bl d11 apto 101</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">brecho kids </t>
+          <t>nanakarana</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Av. das Américas, 29470 </t>
+          <t xml:space="preserve">Estrada dos Bandeirantes, 28131 </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>bl d11 apto 101</t>
+          <t>Galpão 3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -554,34 +558,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>nanakarana</t>
+          <t>Guaracamp</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Estrada dos Bandeirantes, 28131 </t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Galpão 3</t>
-        </is>
-      </c>
+          <t>ESTRADA RIO SAO PAULO 1700</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Guaracamp</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ESTRADA RIO SAO PAULO 1700</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>